<commit_message>
Add precision and data frame
</commit_message>
<xml_diff>
--- a/Analyse/Capteur.xlsx
+++ b/Analyse/Capteur.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJET SN 2020\FFVL\Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Balise_FFVL\Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <t>Unité</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Température</t>
   </si>
   <si>
-    <t>±0,5</t>
-  </si>
-  <si>
     <t>0 à 40</t>
   </si>
   <si>
@@ -119,12 +116,73 @@
   </si>
   <si>
     <t>°</t>
+  </si>
+  <si>
+    <t>Protocole inspiré du NMEA</t>
+  </si>
+  <si>
+    <t>Séparateur de données : Point Virgule</t>
+  </si>
+  <si>
+    <t>Contenu de la trame :</t>
+  </si>
+  <si>
+    <t>Example :</t>
+  </si>
+  <si>
+    <t>Example transmis:</t>
+  </si>
+  <si>
+    <t>Date et Heure</t>
+  </si>
+  <si>
+    <t>4 octets</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>TPM</t>
+  </si>
+  <si>
+    <t>TPM = Taux de Précision Manquant</t>
+  </si>
+  <si>
+    <t>1 octet</t>
+  </si>
+  <si>
+    <t>Nbr octet(s):</t>
+  </si>
+  <si>
+    <t>2 octets</t>
+  </si>
+  <si>
+    <t>±0,8</t>
+  </si>
+  <si>
+    <t>Calcul Nbr octet:</t>
+  </si>
+  <si>
+    <t>Valeur Max</t>
+  </si>
+  <si>
+    <t>Nbr Octet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ? octets</t>
+  </si>
+  <si>
+    <t>? octets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="169" formatCode="dd/mm/yy\ h:mm:ss;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -148,7 +206,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -171,14 +229,393 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,123 +896,238 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="15" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="23" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="G2" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="27" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="G3" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="29">
+        <v>10.5</v>
+      </c>
+      <c r="I3" s="29">
+        <v>500</v>
+      </c>
+      <c r="J3" s="29">
+        <v>15</v>
+      </c>
+      <c r="K3" s="30">
+        <v>43863.11042824074</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E4" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="G4" s="32"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="38"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="G5" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="34">
+        <v>105</v>
+      </c>
+      <c r="I5" s="34">
+        <v>200</v>
+      </c>
+      <c r="J5" s="34">
+        <v>15</v>
+      </c>
+      <c r="K5" s="37">
+        <f>K3</f>
+        <v>43863.11042824074</v>
+      </c>
+      <c r="L5" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E6" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="G6" s="32"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="38"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E7" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="G7" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
@@ -583,36 +1135,167 @@
       <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="E8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="33"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="36"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E10" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E11" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>4</v>
+      <c r="C13" s="4"/>
+      <c r="D13" s="15"/>
+      <c r="O13" s="14"/>
+    </row>
+    <row r="14" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="15"/>
+      <c r="O14" s="14"/>
+    </row>
+    <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="15"/>
+      <c r="O15" s="14"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G17" s="20"/>
+      <c r="J17" s="19"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="24"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="16"/>
+      <c r="J18" s="18"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="18"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <f>2^(8*H21)</f>
+        <v>65536</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="B13:C14"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>